<commit_message>
Fixing search terms file.
</commit_message>
<xml_diff>
--- a/Portal_SearchTerms.xlsx
+++ b/Portal_SearchTerms.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josie\Dropbox\SBBG\Cal_IBIS\Updating Collections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josie\Dropbox\SBBG\Cal_IBIS\Updating Collections\SBBG-Cal-IBIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D2C276-0D6C-44DC-A73D-6B12A45ACB64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDC4E06-49C4-4245-AEC2-14CA7B410FB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10095" yWindow="11700" windowWidth="32775" windowHeight="17445" activeTab="2" xr2:uid="{80AC5E76-7837-4E77-A94B-CD2FC47B468E}"/>
+    <workbookView minimized="1" xWindow="-9570" yWindow="3855" windowWidth="19185" windowHeight="11820" activeTab="4" xr2:uid="{80AC5E76-7837-4E77-A94B-CD2FC47B468E}"/>
   </bookViews>
   <sheets>
     <sheet name="CCH2" sheetId="1" r:id="rId1"/>
     <sheet name="SEINet" sheetId="2" r:id="rId2"/>
     <sheet name="SCAN" sheetId="3" r:id="rId3"/>
+    <sheet name="Ecdysis" sheetId="4" r:id="rId4"/>
+    <sheet name="MyCo Portal" sheetId="5" r:id="rId5"/>
+    <sheet name="CNALH" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="129">
   <si>
     <t>Island</t>
   </si>
@@ -387,6 +390,42 @@
   </si>
   <si>
     <t>Clement Is</t>
+  </si>
+  <si>
+    <t>San Clemente Island</t>
+  </si>
+  <si>
+    <t>San Miguel Island</t>
+  </si>
+  <si>
+    <t>San Nicolas Island</t>
+  </si>
+  <si>
+    <t>Santa Barbara Island</t>
+  </si>
+  <si>
+    <t>San Nicholas Island</t>
+  </si>
+  <si>
+    <t>Cruz Island</t>
+  </si>
+  <si>
+    <t>Rosa Island</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Benito Island</t>
+  </si>
+  <si>
+    <t>Santos Island</t>
+  </si>
+  <si>
+    <t>Isla cedros</t>
+  </si>
+  <si>
+    <t>San Martin</t>
   </si>
 </sst>
 </file>
@@ -448,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -460,6 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,14 +822,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3A5982-CC63-4C8B-A874-756B8CBC4381}">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B74" sqref="B2:C74"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="1" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="57.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
@@ -823,13 +862,13 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>97</v>
+        <v>68</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,13 +879,13 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>97</v>
+        <v>4159</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -854,13 +893,13 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="D4">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>98</v>
@@ -871,16 +910,16 @@
         <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>97</v>
+        <v>10753</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -888,13 +927,13 @@
         <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>4159</v>
+        <v>85</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>98</v>
@@ -905,16 +944,16 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>97</v>
+        <v>4005</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -922,16 +961,16 @@
         <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>97</v>
+        <v>197</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -939,16 +978,16 @@
         <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D9">
-        <v>18</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>97</v>
+        <v>63</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -956,13 +995,13 @@
         <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>6530</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>98</v>
@@ -973,13 +1012,13 @@
         <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>10753</v>
+        <v>1853</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>98</v>
@@ -990,16 +1029,16 @@
         <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,16 +1046,16 @@
         <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="D13">
-        <v>6</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>97</v>
+        <v>284</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1024,13 +1063,13 @@
         <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="D14">
-        <v>85</v>
+        <v>19933</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>98</v>
@@ -1041,16 +1080,16 @@
         <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>97</v>
+        <v>34</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,657 +1097,654 @@
         <v>83</v>
       </c>
       <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>371</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>27320</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>129</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>8139</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20">
+        <v>2648</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21">
+        <v>789</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22">
+        <v>3144</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23">
+        <v>135</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25">
+        <v>321</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26">
+        <v>103</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27">
+        <v>41</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28">
+        <v>194</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29">
+        <v>131</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30">
+        <v>423</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31">
+        <v>73</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32">
+        <v>161</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33">
+        <v>670</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>86</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>23</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36">
+        <v>146</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37">
+        <v>257</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E38" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40">
         <v>2</v>
       </c>
-      <c r="D16">
-        <v>4005</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="E40" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41">
+        <v>12</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43">
+        <v>18</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>6</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" t="s">
         <v>29</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C47" t="s">
         <v>74</v>
       </c>
-      <c r="D17">
+      <c r="D47">
         <v>2</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="E47" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18">
-        <v>197</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C48" t="s">
         <v>71</v>
       </c>
-      <c r="D19">
+      <c r="D48">
         <v>3</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20">
-        <v>63</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22">
-        <v>6530</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23">
-        <v>4</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24">
-        <v>1853</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25">
-        <v>4</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26">
-        <v>60</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27">
-        <v>284</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28">
-        <v>4</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29">
-        <v>19933</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30">
-        <v>7</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31">
-        <v>34</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32">
-        <v>371</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33">
-        <v>27320</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34">
-        <v>5</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35">
-        <v>4</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36">
-        <v>129</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37">
-        <v>8139</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38">
-        <v>7</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39">
-        <v>2</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>84</v>
-      </c>
-      <c r="B40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40">
-        <v>2648</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41">
-        <v>789</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42">
-        <v>6</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43">
-        <v>7</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" t="s">
-        <v>94</v>
-      </c>
-      <c r="D44">
-        <v>2</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45">
-        <v>3144</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46">
-        <v>135</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47">
-        <v>20</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>84</v>
-      </c>
-      <c r="B48" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" t="s">
-        <v>31</v>
-      </c>
-      <c r="D48">
-        <v>321</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F48" t="s">
-        <v>96</v>
+      <c r="E48" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="F49" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C50" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D50">
-        <v>103</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F50" t="s">
-        <v>96</v>
+        <v>4</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="D51">
-        <v>41</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F51" t="s">
-        <v>96</v>
+        <v>4</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D52">
-        <v>194</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>98</v>
+        <v>4</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>97</v>
@@ -1716,16 +1752,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>97</v>
@@ -1733,19 +1769,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="D55">
-        <v>131</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>98</v>
+        <v>4</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1753,13 +1789,13 @@
         <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>97</v>
@@ -1770,10 +1806,10 @@
         <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -1787,16 +1823,16 @@
         <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C58" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="D58">
-        <v>423</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>98</v>
+        <v>6</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1804,16 +1840,16 @@
         <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="D59">
-        <v>73</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>98</v>
+        <v>7</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1821,13 +1857,13 @@
         <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="D60">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>97</v>
@@ -1838,16 +1874,19 @@
         <v>84</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C61" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="D61">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>97</v>
+      </c>
+      <c r="F61" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1855,10 +1894,10 @@
         <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C62" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -1872,13 +1911,13 @@
         <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C63" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>97</v>
@@ -1889,13 +1928,13 @@
         <v>84</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="D64">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>97</v>
@@ -1906,16 +1945,16 @@
         <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C65" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="D65">
-        <v>161</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>98</v>
+        <v>2</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1923,13 +1962,13 @@
         <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C66" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>97</v>
@@ -1940,16 +1979,16 @@
         <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C67" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D67">
-        <v>670</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>98</v>
+        <v>7</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1957,13 +1996,13 @@
         <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C68" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>97</v>
@@ -1974,13 +2013,13 @@
         <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C69" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D69">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>97</v>
@@ -1991,16 +2030,16 @@
         <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C70" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D70">
-        <v>86</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>98</v>
+        <v>18</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2008,16 +2047,16 @@
         <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C71" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D71">
-        <v>23</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>98</v>
+        <v>3</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2025,13 +2064,13 @@
         <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C72" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="D72">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>97</v>
@@ -2045,13 +2084,13 @@
         <v>32</v>
       </c>
       <c r="C73" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D73">
-        <v>146</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>98</v>
+        <v>17</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2062,20 +2101,20 @@
         <v>32</v>
       </c>
       <c r="C74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D74">
-        <v>257</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>98</v>
+        <v>5</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F74">
+    <sortCondition descending="1" ref="E2:E74"/>
     <sortCondition ref="A2:A74"/>
     <sortCondition ref="B2:B74"/>
-    <sortCondition ref="C2:C74"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2086,14 +2125,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94162A4E-1496-4F4F-B244-1BC1D90DB133}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="1" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="57.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
@@ -2138,17 +2176,20 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>97</v>
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F3" s="5"/>
     </row>
@@ -2157,13 +2198,13 @@
         <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D4" s="5">
-        <v>1516</v>
+        <v>7231</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>98</v>
@@ -2172,34 +2213,34 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>97</v>
+        <v>3139</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="D6" s="5">
-        <v>235</v>
+        <v>110</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>98</v>
@@ -2211,16 +2252,16 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D7" s="5">
-        <v>3</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>97</v>
+        <v>4822</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -2229,13 +2270,13 @@
         <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5">
-        <v>37</v>
+        <v>1516</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>98</v>
@@ -2250,10 +2291,10 @@
         <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D9" s="5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>98</v>
@@ -2268,13 +2309,13 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>97</v>
+        <v>36</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F10" s="5"/>
     </row>
@@ -2298,49 +2339,52 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>97</v>
+        <v>12</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>97</v>
+        <v>15</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D14" s="5">
-        <v>1256</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>98</v>
@@ -2352,13 +2396,13 @@
         <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="D15" s="5">
-        <v>10</v>
+        <v>19572</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>98</v>
@@ -2370,49 +2414,49 @@
         <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="D16" s="5">
-        <v>8</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>97</v>
+        <v>6419</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="D17" s="5">
-        <v>5</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>97</v>
+        <v>1256</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="D18" s="5">
-        <v>7231</v>
+        <v>663</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>98</v>
@@ -2420,61 +2464,58 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="5">
         <v>103</v>
       </c>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19" t="s">
-        <v>96</v>
-      </c>
+      <c r="E19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D20" s="5">
-        <v>16</v>
+        <v>1102</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F20" t="s">
-        <v>96</v>
-      </c>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="D21" s="5">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F21" t="s">
-        <v>96</v>
-      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2484,13 +2525,13 @@
         <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" s="5">
-        <v>2</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>97</v>
+        <v>16</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F22" t="s">
         <v>96</v>
@@ -2504,13 +2545,13 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="D23" s="5">
-        <v>8</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>97</v>
+        <v>196</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F23" t="s">
         <v>96</v>
@@ -2521,31 +2562,36 @@
         <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D24" s="5">
-        <v>1</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="D25" s="5">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>97</v>
+        <v>130</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F25" s="5"/>
     </row>
@@ -2554,16 +2600,16 @@
         <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="D26" s="5">
-        <v>2</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>97</v>
+        <v>55</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="F26" s="5"/>
     </row>
@@ -2572,13 +2618,13 @@
         <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D27" s="5">
-        <v>1102</v>
+        <v>235</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>98</v>
@@ -2590,13 +2636,13 @@
         <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D28" s="5">
-        <v>663</v>
+        <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>98</v>
@@ -2608,33 +2654,31 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D29" s="5">
-        <v>25</v>
+        <v>143</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F29" t="s">
-        <v>96</v>
-      </c>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D30" s="5">
-        <v>103</v>
+        <v>404</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>98</v>
@@ -2646,13 +2690,13 @@
         <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
       <c r="D31" s="5">
-        <v>197</v>
+        <v>19</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>98</v>
@@ -2664,13 +2708,13 @@
         <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D32" s="5">
-        <v>130</v>
+        <v>24</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>98</v>
@@ -2682,13 +2726,13 @@
         <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D33" s="5">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>98</v>
@@ -2700,13 +2744,13 @@
         <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="D34" s="5">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>98</v>
@@ -2715,49 +2759,49 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="D35" s="5">
-        <v>19</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>98</v>
+        <v>8</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="D36" s="5">
-        <v>24</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>98</v>
+        <v>5</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
@@ -2769,16 +2813,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="D38" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>97</v>
@@ -2787,16 +2831,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D39" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>97</v>
@@ -2804,14 +2848,17 @@
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="D40" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>97</v>
@@ -2820,19 +2867,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="D41" s="5">
-        <v>404</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F41" s="5"/>
     </row>
@@ -2841,10 +2888,10 @@
         <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D42" s="5">
         <v>1</v>
@@ -2859,16 +2906,16 @@
         <v>83</v>
       </c>
       <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="5">
         <v>1</v>
       </c>
-      <c r="C43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="5">
-        <v>3139</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>98</v>
+      <c r="E43" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F43" s="5"/>
     </row>
@@ -2877,136 +2924,143 @@
         <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D44" s="5">
-        <v>55</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="D45" s="5">
-        <v>110</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>98</v>
+        <v>2</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D46" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F46" s="5"/>
+      <c r="F46" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B47" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D47" s="5">
-        <v>4822</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F47" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D48" s="5">
-        <v>12</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="D49" s="5">
-        <v>15</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D50" s="5">
-        <v>26</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="D51" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>97</v>
@@ -3015,31 +3069,28 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D52" s="5">
-        <v>19572</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>98</v>
+        <v>7</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>83</v>
-      </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="D53" s="5">
         <v>1</v>
@@ -3050,14 +3101,11 @@
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>83</v>
-      </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D54" s="5">
         <v>1</v>
@@ -3068,14 +3116,11 @@
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>83</v>
-      </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="D55" s="5">
         <v>1</v>
@@ -3083,59 +3128,52 @@
       <c r="E55" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F55" s="5"/>
+      <c r="F55" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>83</v>
-      </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="D56" s="5">
-        <v>6419</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>98</v>
+        <v>2</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>84</v>
-      </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C57" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="D57" s="5">
-        <v>123</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>84</v>
-      </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C58" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="D58" s="5">
-        <v>111</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>98</v>
+        <v>1</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="F58" s="5"/>
     </row>
@@ -3149,7 +3187,9 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F58">
-    <sortCondition ref="C2:C58"/>
+    <sortCondition descending="1" ref="E2:E58"/>
+    <sortCondition ref="A2:A58"/>
+    <sortCondition ref="B2:B58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3159,8 +3199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BE95FF-2CC0-4D39-A05E-B57FD1319C95}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3248,13 +3288,13 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>97</v>
+        <v>1247</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3262,13 +3302,13 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D6">
-        <v>1247</v>
+        <v>1052</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>98</v>
@@ -3279,13 +3319,13 @@
         <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="D7">
-        <v>1052</v>
+        <v>2598</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>98</v>
@@ -3296,13 +3336,13 @@
         <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="D8">
-        <v>2598</v>
+        <v>14711</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>98</v>
@@ -3310,16 +3350,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D9">
-        <v>14711</v>
+        <v>474</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>98</v>
@@ -3330,13 +3370,13 @@
         <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="D10">
-        <v>474</v>
+        <v>294</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>98</v>
@@ -3347,13 +3387,13 @@
         <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D11">
-        <v>294</v>
+        <v>82</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>98</v>
@@ -3364,13 +3404,13 @@
         <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="D12">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>98</v>
@@ -3381,16 +3421,16 @@
         <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>97</v>
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3398,13 +3438,13 @@
         <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D14">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>98</v>
@@ -3415,13 +3455,13 @@
         <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>98</v>
@@ -3429,16 +3469,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>97</v>
@@ -3449,16 +3489,16 @@
         <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="D17">
-        <v>40</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>98</v>
+        <v>2</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3466,19 +3506,1062 @@
         <v>106</v>
       </c>
       <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E18">
+    <sortCondition descending="1" ref="E2:E18"/>
+    <sortCondition ref="A2:A18"/>
+    <sortCondition ref="B2:B18"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493BCC14-C6B5-4911-8CBD-4841D0D10907}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>460</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3">
+        <v>1421</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4">
+        <v>1656</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5">
+        <v>1395</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7">
+        <v>389</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8">
+        <v>1416</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9">
+        <v>5673</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10">
+        <v>2794</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D18">
-        <v>16</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>98</v>
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AEE462-65F5-4111-ACD2-1DBB76FD5CC8}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12">
+        <v>39</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13">
+        <v>75</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14">
+        <v>113</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15">
+        <v>180</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16">
+        <v>242</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17">
+        <v>291</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18">
+        <v>716</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19">
+        <v>965</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E19">
+    <sortCondition ref="D2:D19"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EDEA7A-FD4F-4B2C-BFC1-FA871B5374C9}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="6">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="6">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="6">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="6">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="6">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="6">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="6">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="6">
+        <v>165</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="6">
+        <v>251</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6">
+        <v>617</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="6">
+        <v>650</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="6">
+        <v>987</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1054</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1147</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1325</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="6">
+        <v>2153</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2831</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3582</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3803</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E20">
+    <sortCondition ref="D2:D20"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>